<commit_message>
fix: :memo: update excel
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adao_jr/Documents/GIT/Trybe/Projetos/1.Proj_Trybe/sd-010-b-mysql-one-for-all/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB99E8F-2528-F246-A5D9-ADA9350D2439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="1960" yWindow="1180" windowWidth="18920" windowHeight="18380" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="ORIGINAL" sheetId="1" r:id="rId1"/>
+    <sheet name="USUARIOS" sheetId="4" r:id="rId2"/>
+    <sheet name="PLANOS" sheetId="3" r:id="rId3"/>
+    <sheet name="ALBUNS" sheetId="2" r:id="rId4"/>
+    <sheet name="ARTISTAS" sheetId="6" r:id="rId5"/>
+    <sheet name="MUSICAS" sheetId="7" r:id="rId6"/>
+    <sheet name="SEGUINDO" sheetId="5" r:id="rId7"/>
+    <sheet name="REPRODUCOES" sheetId="8" r:id="rId8"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="123">
   <si>
     <t>usuario_id</t>
   </si>
@@ -128,33 +144,272 @@
   </si>
   <si>
     <t>"Thang Of Thunder", "Words Of Her Life", "Without My Streets"</t>
+  </si>
+  <si>
+    <t>plano_id</t>
+  </si>
+  <si>
+    <t>historico_reproducoes</t>
+  </si>
+  <si>
+    <t>artista_id</t>
+  </si>
+  <si>
+    <t>musica_id</t>
+  </si>
+  <si>
+    <t>musica</t>
+  </si>
+  <si>
+    <t>"Soul For Us"</t>
+  </si>
+  <si>
+    <t>"Reflections Of Magic"</t>
+  </si>
+  <si>
+    <t>"Dance With Her Own"</t>
+  </si>
+  <si>
+    <t>"Troubles Of My Inner Fire"</t>
+  </si>
+  <si>
+    <t>"Time Fireworks"</t>
+  </si>
+  <si>
+    <t>"Magic Circus"</t>
+  </si>
+  <si>
+    <t>"Honey, So Do I"</t>
+  </si>
+  <si>
+    <t>"Sweetie, Let's Go Wild"</t>
+  </si>
+  <si>
+    <t>"She Knows"</t>
+  </si>
+  <si>
+    <t>"Fantasy For Me"</t>
+  </si>
+  <si>
+    <t>"Celebration Of More"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Rock His Everything"</t>
+  </si>
+  <si>
+    <t>"Home Forever"</t>
+  </si>
+  <si>
+    <t>"Diamond Power"</t>
+  </si>
+  <si>
+    <t>"Honey, Let's Be Silly"</t>
+  </si>
+  <si>
+    <t>"Thang Of Thunder"</t>
+  </si>
+  <si>
+    <t>"Words Of Her Life"</t>
+  </si>
+  <si>
+    <t>"Without My Streets"</t>
+  </si>
+  <si>
+    <t>('Walter Phoenix'),</t>
+  </si>
+  <si>
+    <t>('Peter Strong'),</t>
+  </si>
+  <si>
+    <t>('Lance Day'),</t>
+  </si>
+  <si>
+    <t>('Freedie Shannon');</t>
+  </si>
+  <si>
+    <t>('Soul For Us',</t>
+  </si>
+  <si>
+    <t>1),</t>
+  </si>
+  <si>
+    <t>2),</t>
+  </si>
+  <si>
+    <t>3),</t>
+  </si>
+  <si>
+    <t>4),</t>
+  </si>
+  <si>
+    <t>5),</t>
+  </si>
+  <si>
+    <t>5);</t>
+  </si>
+  <si>
+    <t>('Reflections Of Magic',</t>
+  </si>
+  <si>
+    <t>('Dance With Her Own',</t>
+  </si>
+  <si>
+    <t>('Troubles Of My Inner Fire',</t>
+  </si>
+  <si>
+    <t>('Time Fireworks',</t>
+  </si>
+  <si>
+    <t>('Magic Circus',</t>
+  </si>
+  <si>
+    <t>('Honey, So Do I',</t>
+  </si>
+  <si>
+    <t>('She Knows',</t>
+  </si>
+  <si>
+    <t>('Fantasy For Me',</t>
+  </si>
+  <si>
+    <t>('Celebration Of More',</t>
+  </si>
+  <si>
+    <t>('Rock His Everything',</t>
+  </si>
+  <si>
+    <t>('Home Forever',</t>
+  </si>
+  <si>
+    <t>('Diamond Power',</t>
+  </si>
+  <si>
+    <t>('Thang Of Thunder',</t>
+  </si>
+  <si>
+    <t>('Words Of Her Life',</t>
+  </si>
+  <si>
+    <t>('Without My Streets',</t>
+  </si>
+  <si>
+    <t>(1,</t>
+  </si>
+  <si>
+    <t>(2,</t>
+  </si>
+  <si>
+    <t>(3,</t>
+  </si>
+  <si>
+    <t>(4,</t>
+  </si>
+  <si>
+    <t>4);</t>
+  </si>
+  <si>
+    <t>6),</t>
+  </si>
+  <si>
+    <t>14),</t>
+  </si>
+  <si>
+    <t>16),</t>
+  </si>
+  <si>
+    <t>13),</t>
+  </si>
+  <si>
+    <t>17),</t>
+  </si>
+  <si>
+    <t>15),</t>
+  </si>
+  <si>
+    <t>18),</t>
+  </si>
+  <si>
+    <t>11);</t>
+  </si>
+  <si>
+    <t>0),</t>
+  </si>
+  <si>
+    <t>7,99),</t>
+  </si>
+  <si>
+    <t>5,99);</t>
+  </si>
+  <si>
+    <t>23,</t>
+  </si>
+  <si>
+    <t>35,</t>
+  </si>
+  <si>
+    <t>20,</t>
+  </si>
+  <si>
+    <t>45,</t>
+  </si>
+  <si>
+    <t>("Honey, Let's Be Silly",</t>
+  </si>
+  <si>
+    <t>("Sweetie, Let's Go Wild",</t>
+  </si>
+  <si>
+    <t>1);</t>
+  </si>
+  <si>
+    <t>('Envious',</t>
+  </si>
+  <si>
+    <t>('Exuberant',</t>
+  </si>
+  <si>
+    <t>('Hallowed Steam',</t>
+  </si>
+  <si>
+    <t>('Incandescent',</t>
+  </si>
+  <si>
+    <t>('Temporary Culture',</t>
+  </si>
+  <si>
+    <t>('gratuito',</t>
+  </si>
+  <si>
+    <t>('familiar',</t>
+  </si>
+  <si>
+    <t>('universitário',</t>
+  </si>
+  <si>
+    <t>('Thati',</t>
+  </si>
+  <si>
+    <t>('Cintia',</t>
+  </si>
+  <si>
+    <t>('Bill',</t>
+  </si>
+  <si>
+    <t>('Roger',</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="9"/>
       <name val="Calibri"/>
@@ -186,7 +441,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -362,96 +617,363 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+  <cellXfs count="61">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -461,27 +983,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ff4472c4"/>
-      <rgbColor rgb="ff8eaadb"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffd9e2f3"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FF4472C4"/>
+      <rgbColor rgb="FF8EAADB"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFD9E2F3"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -683,7 +1263,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -702,7 +1282,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -732,7 +1312,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -758,7 +1338,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -784,7 +1364,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -810,7 +1390,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -836,7 +1416,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -862,7 +1442,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -888,7 +1468,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -914,7 +1494,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -940,7 +1520,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -953,9 +1533,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -972,7 +1558,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -991,7 +1577,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1017,7 +1603,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1043,7 +1629,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1069,7 +1655,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1095,7 +1681,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1121,7 +1707,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1147,7 +1733,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1173,7 +1759,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1199,7 +1785,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1225,7 +1811,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1238,9 +1824,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1254,7 +1846,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1273,7 +1865,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1303,7 +1895,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1329,7 +1921,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1355,7 +1947,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1381,7 +1973,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1407,7 +1999,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1433,7 +2025,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1459,7 +2051,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1485,7 +2077,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1511,7 +2103,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1524,172 +2116,182 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.3516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.4688" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="35.1406" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="35.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="38.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.3516" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="24" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="31.5" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="3">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="4">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="5"/>
-      <c r="H1" t="s" s="4">
+      <c r="H1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I1" t="s" s="6">
+      <c r="I1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="30" customHeight="1">
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="8">
+      <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="9">
         <v>23</v>
       </c>
-      <c r="D2" t="s" s="8">
+      <c r="D2" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="9">
         <v>0</v>
       </c>
-      <c r="F2" t="s" s="10">
+      <c r="F2" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="11">
         <v>1</v>
       </c>
-      <c r="I2" t="s" s="12">
+      <c r="I2" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" ht="45" customHeight="1">
+    <row r="3" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="14">
+      <c r="B3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="15">
         <v>35</v>
       </c>
-      <c r="D3" t="s" s="14">
+      <c r="D3" s="14" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="15">
         <v>7.99</v>
       </c>
-      <c r="F3" t="s" s="16">
+      <c r="F3" s="16" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="17"/>
       <c r="H3" s="18">
         <v>2</v>
       </c>
-      <c r="I3" t="s" s="19">
+      <c r="I3" s="19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" ht="31.5" customHeight="1">
+    <row r="4" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="8">
+      <c r="B4" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="9">
         <v>20</v>
       </c>
-      <c r="D4" t="s" s="8">
+      <c r="D4" s="8" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="9">
         <v>5.99</v>
       </c>
-      <c r="F4" t="s" s="10">
+      <c r="F4" s="10" t="s">
         <v>17</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="11">
         <v>3</v>
       </c>
-      <c r="I4" t="s" s="12">
+      <c r="I4" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" ht="39" customHeight="1">
+    <row r="5" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="14">
+      <c r="B5" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="15">
         <v>45</v>
       </c>
-      <c r="D5" t="s" s="14">
+      <c r="D5" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="15">
         <v>0</v>
       </c>
-      <c r="F5" t="s" s="16">
+      <c r="F5" s="16" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="17"/>
       <c r="H5" s="18">
         <v>4</v>
       </c>
-      <c r="I5" t="s" s="19">
+      <c r="I5" s="19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" ht="38.1" customHeight="1">
+    <row r="6" spans="1:9" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="20"/>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
@@ -1700,17 +2302,17 @@
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
     </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="2">
+    <row r="7" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s" s="3">
+      <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s" s="3">
+      <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D7" t="s" s="3">
+      <c r="D7" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="24"/>
@@ -1719,17 +2321,17 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" ht="26.55" customHeight="1">
+    <row r="8" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>1</v>
       </c>
-      <c r="B8" t="s" s="8">
+      <c r="B8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" t="s" s="8">
+      <c r="C8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D8" t="s" s="26">
+      <c r="D8" s="26" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="24"/>
@@ -1738,17 +2340,17 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" ht="13.55" customHeight="1">
+    <row r="9" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>2</v>
       </c>
-      <c r="B9" t="s" s="14">
+      <c r="B9" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C9" t="s" s="14">
+      <c r="C9" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D9" t="s" s="27">
+      <c r="D9" s="27" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="25"/>
@@ -1757,17 +2359,17 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" ht="26.55" customHeight="1">
+    <row r="10" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>3</v>
       </c>
-      <c r="B10" t="s" s="8">
+      <c r="B10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="s" s="8">
+      <c r="C10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D10" t="s" s="26">
+      <c r="D10" s="26" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="24"/>
@@ -1776,17 +2378,17 @@
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
     </row>
-    <row r="11" ht="39.55" customHeight="1">
+    <row r="11" spans="1:9" ht="39.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <v>4</v>
       </c>
-      <c r="B11" t="s" s="14">
+      <c r="B11" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s" s="14">
+      <c r="C11" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D11" t="s" s="27">
+      <c r="D11" s="27" t="s">
         <v>36</v>
       </c>
       <c r="E11" s="25"/>
@@ -1795,17 +2397,17 @@
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
     </row>
-    <row r="12" ht="26.55" customHeight="1">
+    <row r="12" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>5</v>
       </c>
-      <c r="B12" t="s" s="8">
+      <c r="B12" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C12" t="s" s="8">
+      <c r="C12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D12" t="s" s="26">
+      <c r="D12" s="26" t="s">
         <v>38</v>
       </c>
       <c r="E12" s="24"/>
@@ -1816,7 +2418,1197 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B8DC615-1B3C-944B-8582-70644CEFC7CA}">
+  <dimension ref="B1:E7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="0.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="39">
+        <v>1</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="40">
+        <v>2</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="41">
+        <v>3</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="49" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="40">
+        <v>4</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="48" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+  <ignoredErrors>
+    <ignoredError sqref="D3:D6" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C222C7-8778-254A-9B21-4CD981F0C65C}">
+  <dimension ref="B1:D7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="1.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="39">
+        <v>1</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="40">
+        <v>2</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="41">
+        <v>3</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+    </row>
+    <row r="7" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C895E55C-A528-1C43-82F2-53EB96D1DE61}">
+  <dimension ref="B1:E7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="0.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="7" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:5" s="28" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="43">
+        <v>1</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="44">
+        <v>2</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="45">
+        <v>3</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="44">
+        <v>4</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="46">
+        <v>5</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0112360E-3D58-0844-A526-00B8C91EC334}">
+  <dimension ref="B1:C7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="0.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="7" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:3" s="28" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="43">
+        <v>1</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="44">
+        <v>2</v>
+      </c>
+      <c r="C4" s="57" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="45">
+        <v>3</v>
+      </c>
+      <c r="C5" s="58" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="44">
+        <v>4</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="46"/>
+      <c r="C7" s="42"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E33220-3FCD-5B4F-A4D2-07085F224460}">
+  <dimension ref="B1:D21"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="0.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="7" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:4" s="28" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="43">
+        <v>1</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="44">
+        <v>2</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="45">
+        <v>3</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="44">
+        <v>4</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="45">
+        <v>5</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="44">
+        <v>6</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="45">
+        <v>7</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="44">
+        <v>8</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="59" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="45">
+        <v>9</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="60" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="44">
+        <v>10</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="45">
+        <v>11</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="60" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="44">
+        <v>12</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="45">
+        <v>13</v>
+      </c>
+      <c r="C15" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="60" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="44">
+        <v>14</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="45">
+        <v>15</v>
+      </c>
+      <c r="C17" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="60" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="44">
+        <v>16</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="48" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="45">
+        <v>17</v>
+      </c>
+      <c r="C19" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="49" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="44">
+        <v>18</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="48" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="42"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E47391E-F58C-DD4C-8E1F-44923D5FFAAD}">
+  <dimension ref="B1:H11"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="0.83203125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="35" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="2.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="37"/>
+      <c r="G2" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="43">
+        <v>1</v>
+      </c>
+      <c r="H3" s="39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="52"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="51"/>
+    </row>
+    <row r="5" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="52"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="51"/>
+    </row>
+    <row r="6" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="44">
+        <v>2</v>
+      </c>
+      <c r="H6" s="40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="30"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="40"/>
+    </row>
+    <row r="8" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="45">
+        <v>3</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="41"/>
+    </row>
+    <row r="10" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="44">
+        <v>4</v>
+      </c>
+      <c r="H10" s="40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="35"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="42"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D34629-556A-E247-99FF-FCA862CED4F2}">
+  <dimension ref="B1:H31"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="C16" sqref="B3:C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="0.83203125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="64" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="43">
+        <v>1</v>
+      </c>
+      <c r="G3" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="52"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="54"/>
+    </row>
+    <row r="5" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="52"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="54"/>
+    </row>
+    <row r="6" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="52"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="54"/>
+    </row>
+    <row r="7" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="44">
+        <v>2</v>
+      </c>
+      <c r="G7" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="30"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="48"/>
+    </row>
+    <row r="9" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="48"/>
+    </row>
+    <row r="10" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="30"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="48"/>
+    </row>
+    <row r="11" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="45">
+        <v>3</v>
+      </c>
+      <c r="G11" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="49"/>
+    </row>
+    <row r="13" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="49"/>
+    </row>
+    <row r="14" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="44">
+        <v>4</v>
+      </c>
+      <c r="G14" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="55"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="48"/>
+    </row>
+    <row r="16" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="55"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="48"/>
+    </row>
+    <row r="17" spans="2:8" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="35"/>
+      <c r="F17" s="45">
+        <v>5</v>
+      </c>
+      <c r="G17" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F18" s="44">
+        <v>6</v>
+      </c>
+      <c r="G18" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F19" s="45">
+        <v>7</v>
+      </c>
+      <c r="G19" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" s="49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F20" s="44">
+        <v>8</v>
+      </c>
+      <c r="G20" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" s="48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F21" s="45">
+        <v>9</v>
+      </c>
+      <c r="G21" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" s="49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F22" s="44">
+        <v>10</v>
+      </c>
+      <c r="G22" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="H22" s="48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F23" s="45">
+        <v>11</v>
+      </c>
+      <c r="G23" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" s="49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F24" s="44">
+        <v>12</v>
+      </c>
+      <c r="G24" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="H24" s="48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F25" s="45">
+        <v>13</v>
+      </c>
+      <c r="G25" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25" s="49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F26" s="44">
+        <v>14</v>
+      </c>
+      <c r="G26" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="H26" s="48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F27" s="45">
+        <v>15</v>
+      </c>
+      <c r="G27" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="H27" s="49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F28" s="44">
+        <v>16</v>
+      </c>
+      <c r="G28" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="H28" s="48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F29" s="45">
+        <v>17</v>
+      </c>
+      <c r="G29" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="H29" s="49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F30" s="44">
+        <v>18</v>
+      </c>
+      <c r="G30" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="H30" s="48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="42"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
fix: :bug: fixes historico_reproducao and seguindo tables in excel/ adds database structure file made in draw.io
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t xml:space="preserve">usuario_id</t>
   </si>
@@ -38,12 +38,6 @@
   </si>
   <si>
     <t xml:space="preserve">artista</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seguindo_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reproducao_id</t>
   </si>
   <si>
     <t xml:space="preserve">cancao_id</t>
@@ -186,7 +180,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -222,11 +216,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -311,7 +300,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -348,7 +337,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -360,7 +349,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -376,7 +365,7 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -398,10 +387,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -484,7 +469,7 @@
   <dimension ref="A1:U41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topLeft" activeCell="M29" activeCellId="0" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -501,7 +486,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.67"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="24.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="19.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="36.31"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="16" min="16" style="1" width="8.85"/>
@@ -533,24 +518,20 @@
       </c>
       <c r="H1" s="0"/>
       <c r="I1" s="4" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>4</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="K1" s="0"/>
       <c r="L1" s="0"/>
       <c r="M1" s="4" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>8</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="O1" s="0"/>
       <c r="Q1" s="0"/>
       <c r="U1" s="0"/>
     </row>
@@ -559,20 +540,20 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>23</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" s="0"/>
       <c r="F2" s="8" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H2" s="0"/>
       <c r="I2" s="8" t="n">
@@ -581,9 +562,7 @@
       <c r="J2" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="K2" s="8" t="n">
-        <v>1</v>
-      </c>
+      <c r="K2" s="0"/>
       <c r="L2" s="0"/>
       <c r="M2" s="8" t="n">
         <v>1</v>
@@ -591,9 +570,7 @@
       <c r="N2" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="O2" s="8" t="n">
-        <v>1</v>
-      </c>
+      <c r="O2" s="0"/>
       <c r="Q2" s="0"/>
       <c r="U2" s="10"/>
     </row>
@@ -602,41 +579,37 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" s="5" t="n">
         <v>35</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" s="0"/>
       <c r="F3" s="8" t="n">
         <v>2</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H3" s="0"/>
       <c r="I3" s="8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" s="8" t="n">
-        <v>4</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="K3" s="0"/>
       <c r="L3" s="0"/>
       <c r="M3" s="8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N3" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="O3" s="8" t="n">
         <v>6</v>
       </c>
+      <c r="O3" s="0"/>
       <c r="Q3" s="0"/>
       <c r="U3" s="11"/>
     </row>
@@ -645,41 +618,37 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="5" t="n">
         <v>20</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4" s="0"/>
       <c r="F4" s="8" t="n">
         <v>3</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H4" s="0"/>
       <c r="I4" s="8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="8" t="n">
-        <v>3</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="K4" s="0"/>
       <c r="L4" s="0"/>
       <c r="M4" s="8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" s="8" t="n">
         <v>14</v>
       </c>
+      <c r="O4" s="0"/>
       <c r="Q4" s="0"/>
       <c r="U4" s="10"/>
     </row>
@@ -688,41 +657,37 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>45</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E5" s="0"/>
       <c r="F5" s="8" t="n">
         <v>4</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H5" s="0"/>
       <c r="I5" s="8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J5" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="K5" s="8" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K5" s="0"/>
       <c r="L5" s="0"/>
       <c r="M5" s="8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N5" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" s="8" t="n">
         <v>16</v>
       </c>
+      <c r="O5" s="0"/>
       <c r="Q5" s="0"/>
       <c r="U5" s="11"/>
     </row>
@@ -736,160 +701,144 @@
       <c r="G6" s="0"/>
       <c r="H6" s="0"/>
       <c r="I6" s="13" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J6" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="K6" s="13" t="n">
-        <v>3</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="K6" s="0"/>
       <c r="M6" s="13" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N6" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="O6" s="13" t="n">
         <v>13</v>
       </c>
+      <c r="O6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="22.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="0"/>
       <c r="E7" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H7" s="0"/>
       <c r="I7" s="8" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J7" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="K7" s="8" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="K7" s="0"/>
       <c r="M7" s="13" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N7" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="O7" s="13" t="n">
         <v>17</v>
       </c>
+      <c r="O7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="26.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>1</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D8" s="0"/>
       <c r="E8" s="8" t="n">
         <v>1</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G8" s="8" t="n">
         <v>1</v>
       </c>
       <c r="H8" s="0"/>
       <c r="I8" s="8" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J8" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="K8" s="8" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K8" s="0"/>
       <c r="M8" s="13" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="N8" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="O8" s="13" t="n">
-        <v>2</v>
-      </c>
+      <c r="O8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="27.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>2</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D9" s="0"/>
       <c r="E9" s="8" t="n">
         <v>2</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G9" s="8" t="n">
         <v>1</v>
       </c>
       <c r="H9" s="0"/>
       <c r="I9" s="8" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J9" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="K9" s="8" t="n">
-        <v>4</v>
-      </c>
+      <c r="K9" s="0"/>
       <c r="M9" s="13" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="N9" s="13" t="n">
-        <v>2</v>
-      </c>
-      <c r="O9" s="13" t="n">
         <v>15</v>
       </c>
+      <c r="O9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="37.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
         <v>3</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D10" s="0"/>
       <c r="E10" s="8" t="n">
         <v>3</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G10" s="8" t="n">
         <v>1</v>
@@ -899,31 +848,29 @@
       <c r="J10" s="0"/>
       <c r="K10" s="0"/>
       <c r="M10" s="13" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="N10" s="13" t="n">
-        <v>3</v>
-      </c>
-      <c r="O10" s="13" t="n">
-        <v>4</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="O10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="n">
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" s="0"/>
       <c r="E11" s="8" t="n">
         <v>4</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G11" s="8" t="n">
         <v>2</v>
@@ -931,32 +878,30 @@
       <c r="H11" s="0"/>
       <c r="I11" s="0"/>
       <c r="J11" s="0"/>
-      <c r="M11" s="13" t="n">
-        <v>10</v>
+      <c r="M11" s="8" t="n">
+        <v>3</v>
       </c>
       <c r="N11" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="O11" s="8" t="n">
         <v>16</v>
       </c>
+      <c r="O11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="26.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="n">
         <v>5</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D12" s="0"/>
       <c r="E12" s="8" t="n">
         <v>5</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G12" s="8" t="n">
         <v>2</v>
@@ -964,22 +909,20 @@
       <c r="H12" s="0"/>
       <c r="I12" s="0"/>
       <c r="J12" s="0"/>
-      <c r="M12" s="13" t="n">
-        <v>11</v>
+      <c r="M12" s="8" t="n">
+        <v>3</v>
       </c>
       <c r="N12" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="O12" s="8" t="n">
         <v>6</v>
       </c>
+      <c r="O12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E13" s="13" t="n">
         <v>6</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G13" s="8" t="n">
         <v>3</v>
@@ -987,51 +930,47 @@
       <c r="H13" s="0"/>
       <c r="I13" s="0"/>
       <c r="J13" s="0"/>
-      <c r="M13" s="13" t="n">
-        <v>12</v>
+      <c r="M13" s="8" t="n">
+        <v>4</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="O13" s="8" t="n">
-        <v>3</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="O13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E14" s="13" t="n">
         <v>7</v>
       </c>
       <c r="F14" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="I14" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="J14" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="K14" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="M14" s="13" t="n">
-        <v>13</v>
+      <c r="M14" s="8" t="n">
+        <v>4</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="O14" s="8" t="n">
         <v>18</v>
       </c>
+      <c r="O14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E15" s="13" t="n">
         <v>8</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G15" s="8" t="n">
         <v>3</v>
@@ -1040,27 +979,25 @@
         <v>1</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K15" s="13" t="n">
         <v>0</v>
       </c>
-      <c r="M15" s="13" t="n">
-        <v>14</v>
+      <c r="M15" s="8" t="n">
+        <v>4</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="O15" s="8" t="n">
         <v>11</v>
       </c>
+      <c r="O15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E16" s="13" t="n">
         <v>9</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G16" s="8" t="n">
         <v>3</v>
@@ -1069,7 +1006,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K16" s="13" t="n">
         <v>7.99</v>
@@ -1081,7 +1018,7 @@
         <v>10</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G17" s="13" t="n">
         <v>4</v>
@@ -1090,7 +1027,7 @@
         <v>3</v>
       </c>
       <c r="J17" s="21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K17" s="13" t="n">
         <v>5.99</v>
@@ -1102,7 +1039,7 @@
         <v>11</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G18" s="13" t="n">
         <v>4</v>
@@ -1111,7 +1048,7 @@
     <row r="19" customFormat="false" ht="15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D19" s="0"/>
       <c r="E19" s="13"/>
-      <c r="F19" s="22"/>
+      <c r="F19" s="16"/>
       <c r="G19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1120,7 +1057,7 @@
         <v>12</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G20" s="13" t="n">
         <v>4</v>
@@ -1132,7 +1069,7 @@
         <v>13</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G21" s="13" t="n">
         <v>4</v>
@@ -1144,7 +1081,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G22" s="13" t="n">
         <v>4</v>
@@ -1157,7 +1094,7 @@
         <v>15</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G23" s="13" t="n">
         <v>4</v>
@@ -1169,7 +1106,7 @@
         <v>16</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G24" s="13" t="n">
         <v>5</v>
@@ -1181,7 +1118,7 @@
         <v>17</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G25" s="13" t="n">
         <v>5</v>
@@ -1193,7 +1130,7 @@
         <v>18</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G26" s="13" t="n">
         <v>5</v>

</xml_diff>